<commit_message>
Added week 6 functions
</commit_message>
<xml_diff>
--- a/Functions for EPID 674.xlsx
+++ b/Functions for EPID 674.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\Research\EPID 674\EPID674_Week1_Class\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE60C4E8-87A2-4EFD-96EB-B674AF2D80A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFA7C1A4-8A9A-40AF-9F71-6F90DB20A4E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{7F09A9C1-C8D2-49BC-9C70-D9B3D5D515C7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="6" xr2:uid="{7F09A9C1-C8D2-49BC-9C70-D9B3D5D515C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="Week 3" sheetId="5" r:id="rId3"/>
     <sheet name="Week 4" sheetId="3" r:id="rId4"/>
     <sheet name="Week 5" sheetId="6" r:id="rId5"/>
-    <sheet name="Compiled Functions" sheetId="4" r:id="rId6"/>
+    <sheet name="Week 6" sheetId="7" r:id="rId6"/>
+    <sheet name="Compiled Functions" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="207">
   <si>
     <t>Function</t>
   </si>
@@ -563,12 +564,6 @@
     <t>Plot the correlation values</t>
   </si>
   <si>
-    <t>corrplot.mixed()</t>
-  </si>
-  <si>
-    <t>corrplot</t>
-  </si>
-  <si>
     <t>t.test()</t>
   </si>
   <si>
@@ -611,16 +606,61 @@
     <t>Create plots with options including: geom_histogram, geom_bar, geom_boxplot, geom_point, geom_violin, geom_pointrange</t>
   </si>
   <si>
-    <t>mhor()</t>
-  </si>
-  <si>
-    <t>tab1()</t>
-  </si>
-  <si>
-    <t>tabpct()</t>
-  </si>
-  <si>
     <t>epiDisplay</t>
+  </si>
+  <si>
+    <t>Calculate odds ratio from 2x2 table</t>
+  </si>
+  <si>
+    <t>lm()</t>
+  </si>
+  <si>
+    <t>par()</t>
+  </si>
+  <si>
+    <t>Set the parameters for a plot</t>
+  </si>
+  <si>
+    <t>glance()</t>
+  </si>
+  <si>
+    <t>broom</t>
+  </si>
+  <si>
+    <t>tidy()</t>
+  </si>
+  <si>
+    <t>Linear regression</t>
+  </si>
+  <si>
+    <t>Get information about regression results</t>
+  </si>
+  <si>
+    <t>Summarise regression results</t>
+  </si>
+  <si>
+    <t>as.formula()</t>
+  </si>
+  <si>
+    <t>Write a formula as a character string</t>
+  </si>
+  <si>
+    <t>stargazer</t>
+  </si>
+  <si>
+    <t>stargazer()</t>
+  </si>
+  <si>
+    <t>Compare regression results from different models</t>
+  </si>
+  <si>
+    <t>pull()</t>
+  </si>
+  <si>
+    <t>dplyr</t>
+  </si>
+  <si>
+    <t>Turn a column into a vector</t>
   </si>
 </sst>
 </file>
@@ -1904,7 +1944,7 @@
         <v>158</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -1947,10 +1987,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FD4E31F-E0A8-46F9-B33A-ECC8DE1813C5}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2009,10 +2049,10 @@
         <v>174</v>
       </c>
       <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" t="s">
         <v>175</v>
-      </c>
-      <c r="C5" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -2034,23 +2074,23 @@
         <v>60</v>
       </c>
       <c r="C7" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B8" t="s">
         <v>60</v>
       </c>
       <c r="C8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B9" t="s">
         <v>60</v>
@@ -2064,7 +2104,7 @@
         <v>184</v>
       </c>
       <c r="B10" t="s">
-        <v>60</v>
+        <v>171</v>
       </c>
       <c r="C10" t="s">
         <v>185</v>
@@ -2072,45 +2112,13 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="B11" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>186</v>
-      </c>
-      <c r="B12" t="s">
-        <v>171</v>
-      </c>
-      <c r="C12" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>191</v>
-      </c>
-      <c r="B13" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
         <v>188</v>
       </c>
-      <c r="B14" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>190</v>
-      </c>
-      <c r="B15" t="s">
-        <v>193</v>
+      <c r="C11" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -2119,12 +2127,120 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCDA47AD-0A41-47D2-B549-B1C29EC7716B}">
-  <dimension ref="A1:C76"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C85972F4-683A-4B9B-B14E-B9E927D74C6E}">
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
+      <selection activeCell="C8" sqref="A2:C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="16.36328125" customWidth="1"/>
+    <col min="3" max="3" width="43.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B4" t="s">
+        <v>194</v>
+      </c>
+      <c r="C4" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>195</v>
+      </c>
+      <c r="B5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>199</v>
+      </c>
+      <c r="B6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>202</v>
+      </c>
+      <c r="B7" t="s">
+        <v>201</v>
+      </c>
+      <c r="C7" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>204</v>
+      </c>
+      <c r="B8" t="s">
+        <v>205</v>
+      </c>
+      <c r="C8" t="s">
+        <v>206</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCDA47AD-0A41-47D2-B549-B1C29EC7716B}">
+  <dimension ref="A1:C92"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2147,832 +2263,1008 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>121</v>
+        <v>179</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
-        <v>122</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>134</v>
+        <v>178</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="C3" t="s">
-        <v>135</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>114</v>
+        <v>134</v>
       </c>
       <c r="B5" t="s">
-        <v>112</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>117</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>199</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>138</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>62</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>114</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>112</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>67</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>123</v>
+        <v>186</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>188</v>
       </c>
       <c r="C11" t="s">
-        <v>124</v>
+        <v>189</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>68</v>
+        <v>184</v>
       </c>
       <c r="B12" t="s">
-        <v>69</v>
+        <v>171</v>
       </c>
       <c r="C12" t="s">
-        <v>70</v>
+        <v>185</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>69</v>
+        <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>72</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>66</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>156</v>
+        <v>34</v>
       </c>
       <c r="B15" t="s">
-        <v>154</v>
+        <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>157</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>123</v>
       </c>
       <c r="B16" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="C16" t="s">
-        <v>37</v>
+        <v>169</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>126</v>
+        <v>168</v>
       </c>
       <c r="B17" t="s">
-        <v>127</v>
+        <v>60</v>
       </c>
       <c r="C17" t="s">
-        <v>129</v>
+        <v>169</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="B18" t="s">
-        <v>4</v>
+        <v>69</v>
       </c>
       <c r="C18" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="C19" t="s">
-        <v>48</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>136</v>
+        <v>23</v>
       </c>
       <c r="B20" t="s">
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>137</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="B21" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="C21" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>159</v>
+        <v>36</v>
       </c>
       <c r="B22" t="s">
-        <v>158</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>189</v>
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>160</v>
+        <v>126</v>
       </c>
       <c r="B23" t="s">
-        <v>158</v>
+        <v>127</v>
       </c>
       <c r="C23" t="s">
-        <v>161</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>107</v>
+        <v>57</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>109</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B25" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="C25" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>21</v>
+        <v>136</v>
       </c>
       <c r="B26" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>22</v>
+        <v>137</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>165</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>166</v>
       </c>
       <c r="C27" t="s">
-        <v>28</v>
+        <v>167</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>149</v>
+        <v>170</v>
       </c>
       <c r="B28" t="s">
-        <v>150</v>
+        <v>172</v>
       </c>
       <c r="C28" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>99</v>
+        <v>159</v>
       </c>
       <c r="B29" t="s">
-        <v>60</v>
-      </c>
-      <c r="C29" t="s">
-        <v>101</v>
+        <v>158</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>51</v>
+        <v>160</v>
       </c>
       <c r="B30" t="s">
-        <v>45</v>
+        <v>158</v>
       </c>
       <c r="C30" t="s">
-        <v>52</v>
+        <v>161</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>10</v>
+        <v>193</v>
       </c>
       <c r="B31" t="s">
-        <v>4</v>
+        <v>194</v>
       </c>
       <c r="C31" t="s">
-        <v>11</v>
+        <v>197</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>3</v>
+        <v>107</v>
       </c>
       <c r="B32" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="C32" t="s">
-        <v>5</v>
+        <v>109</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="B33" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C33" t="s">
-        <v>80</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>84</v>
+        <v>21</v>
       </c>
       <c r="B34" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C34" t="s">
-        <v>86</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>130</v>
+        <v>25</v>
       </c>
       <c r="B35" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="C35" t="s">
-        <v>131</v>
+        <v>28</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>100</v>
+        <v>149</v>
       </c>
       <c r="B36" t="s">
-        <v>4</v>
+        <v>150</v>
       </c>
       <c r="C36" t="s">
-        <v>103</v>
+        <v>151</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B37" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="C37" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>98</v>
+        <v>51</v>
       </c>
       <c r="B38" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="C38" t="s">
-        <v>105</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>95</v>
+        <v>10</v>
       </c>
       <c r="B39" t="s">
         <v>4</v>
       </c>
       <c r="C39" t="s">
-        <v>102</v>
+        <v>11</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="B40" t="s">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="C40" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>119</v>
+        <v>190</v>
       </c>
       <c r="B41" t="s">
         <v>60</v>
       </c>
       <c r="C41" t="s">
-        <v>120</v>
+        <v>196</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>125</v>
+        <v>76</v>
       </c>
       <c r="B42" t="s">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="C42" t="s">
-        <v>128</v>
+        <v>80</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>132</v>
+        <v>84</v>
       </c>
       <c r="B43" t="s">
         <v>4</v>
       </c>
       <c r="C43" t="s">
-        <v>133</v>
+        <v>86</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>27</v>
+        <v>130</v>
       </c>
       <c r="B44" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="C44" t="s">
-        <v>30</v>
+        <v>131</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>146</v>
+        <v>100</v>
       </c>
       <c r="B45" t="s">
         <v>4</v>
       </c>
       <c r="C45" t="s">
-        <v>147</v>
+        <v>103</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>153</v>
+        <v>97</v>
       </c>
       <c r="B46" t="s">
-        <v>154</v>
+        <v>4</v>
       </c>
       <c r="C46" t="s">
-        <v>155</v>
+        <v>106</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>162</v>
+        <v>98</v>
       </c>
       <c r="B47" t="s">
-        <v>163</v>
+        <v>60</v>
       </c>
       <c r="C47" t="s">
-        <v>164</v>
+        <v>105</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>148</v>
+        <v>95</v>
       </c>
       <c r="B48" t="s">
-        <v>150</v>
+        <v>4</v>
       </c>
       <c r="C48" t="s">
-        <v>152</v>
+        <v>102</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="B49" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="C49" t="s">
-        <v>7</v>
+        <v>61</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>81</v>
+        <v>119</v>
       </c>
       <c r="B50" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="C50" t="s">
-        <v>82</v>
+        <v>120</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>96</v>
+        <v>125</v>
       </c>
       <c r="B51" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="C51" t="s">
-        <v>104</v>
+        <v>128</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>75</v>
+        <v>132</v>
       </c>
       <c r="B52" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C52" t="s">
-        <v>78</v>
+        <v>133</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="B53" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="C53" t="s">
-        <v>64</v>
+        <v>30</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>59</v>
+        <v>182</v>
       </c>
       <c r="B54" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C54" t="s">
-        <v>65</v>
+        <v>183</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>31</v>
+        <v>191</v>
       </c>
       <c r="B55" t="s">
-        <v>32</v>
+        <v>150</v>
       </c>
       <c r="C55" t="s">
-        <v>33</v>
+        <v>192</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>49</v>
+        <v>146</v>
       </c>
       <c r="B56" t="s">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="C56" t="s">
-        <v>50</v>
+        <v>147</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>14</v>
+        <v>153</v>
       </c>
       <c r="B57" t="s">
-        <v>4</v>
+        <v>154</v>
       </c>
       <c r="C57" t="s">
-        <v>15</v>
+        <v>155</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>38</v>
+        <v>162</v>
       </c>
       <c r="B58" t="s">
-        <v>4</v>
+        <v>163</v>
       </c>
       <c r="C58" t="s">
-        <v>39</v>
+        <v>164</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>74</v>
+        <v>148</v>
       </c>
       <c r="B59" t="s">
-        <v>4</v>
+        <v>150</v>
       </c>
       <c r="C59" t="s">
-        <v>79</v>
+        <v>152</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>116</v>
+        <v>6</v>
       </c>
       <c r="B60" t="s">
-        <v>115</v>
+        <v>4</v>
       </c>
       <c r="C60" t="s">
-        <v>118</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>90</v>
+        <v>204</v>
       </c>
       <c r="B61" t="s">
-        <v>60</v>
+        <v>205</v>
       </c>
       <c r="C61" t="s">
-        <v>92</v>
+        <v>206</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B62" t="s">
         <v>4</v>
       </c>
       <c r="C62" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>44</v>
+        <v>96</v>
       </c>
       <c r="B63" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C63" t="s">
-        <v>46</v>
+        <v>104</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="B64" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C64" t="s">
-        <v>13</v>
+        <v>78</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>87</v>
+        <v>58</v>
       </c>
       <c r="B65" t="s">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="C65" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>17</v>
+        <v>59</v>
       </c>
       <c r="B66" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="C66" t="s">
-        <v>19</v>
+        <v>65</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>93</v>
+        <v>31</v>
       </c>
       <c r="B67" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C67" t="s">
-        <v>94</v>
+        <v>33</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>89</v>
+        <v>49</v>
       </c>
       <c r="B68" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="C68" t="s">
-        <v>91</v>
+        <v>50</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>142</v>
+        <v>14</v>
       </c>
       <c r="B69" t="s">
         <v>4</v>
       </c>
       <c r="C69" t="s">
-        <v>143</v>
+        <v>15</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="B70" t="s">
         <v>4</v>
       </c>
       <c r="C70" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>111</v>
+        <v>74</v>
       </c>
       <c r="B71" t="s">
-        <v>112</v>
+        <v>4</v>
       </c>
       <c r="C71" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="B72" t="s">
-        <v>4</v>
+        <v>115</v>
       </c>
       <c r="C72" t="s">
-        <v>145</v>
+        <v>118</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="B73" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C73" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>42</v>
+        <v>83</v>
       </c>
       <c r="B74" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C74" t="s">
-        <v>43</v>
+        <v>85</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>140</v>
+        <v>44</v>
       </c>
       <c r="B75" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="C75" t="s">
-        <v>141</v>
+        <v>46</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
+        <v>12</v>
+      </c>
+      <c r="B76" t="s">
+        <v>4</v>
+      </c>
+      <c r="C76" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>87</v>
+      </c>
+      <c r="B77" t="s">
+        <v>20</v>
+      </c>
+      <c r="C77" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>202</v>
+      </c>
+      <c r="B78" t="s">
+        <v>201</v>
+      </c>
+      <c r="C78" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>17</v>
+      </c>
+      <c r="B79" t="s">
+        <v>20</v>
+      </c>
+      <c r="C79" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>93</v>
+      </c>
+      <c r="B80" t="s">
+        <v>45</v>
+      </c>
+      <c r="C80" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>89</v>
+      </c>
+      <c r="B81" t="s">
+        <v>4</v>
+      </c>
+      <c r="C81" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>142</v>
+      </c>
+      <c r="B82" t="s">
+        <v>4</v>
+      </c>
+      <c r="C82" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>174</v>
+      </c>
+      <c r="B83" t="s">
+        <v>60</v>
+      </c>
+      <c r="C83" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>53</v>
+      </c>
+      <c r="B84" t="s">
+        <v>4</v>
+      </c>
+      <c r="C84" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>111</v>
+      </c>
+      <c r="B85" t="s">
+        <v>112</v>
+      </c>
+      <c r="C85" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>195</v>
+      </c>
+      <c r="B86" t="s">
+        <v>194</v>
+      </c>
+      <c r="C86" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>144</v>
+      </c>
+      <c r="B87" t="s">
+        <v>4</v>
+      </c>
+      <c r="C87" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>108</v>
+      </c>
+      <c r="B88" t="s">
+        <v>45</v>
+      </c>
+      <c r="C88" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>42</v>
+      </c>
+      <c r="B89" t="s">
+        <v>20</v>
+      </c>
+      <c r="C89" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>140</v>
+      </c>
+      <c r="B90" t="s">
+        <v>4</v>
+      </c>
+      <c r="C90" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>176</v>
+      </c>
+      <c r="B91" t="s">
+        <v>60</v>
+      </c>
+      <c r="C91" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
         <v>73</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B92" t="s">
         <v>20</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C92" t="s">
         <v>77</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C76">
-    <sortCondition ref="A1:A76"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C92">
+    <sortCondition ref="A1:A92"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>